<commit_message>
mise en plade du rarport mensuel et maj des exports excels
</commit_message>
<xml_diff>
--- a/www/asso_adhesion.xlsx
+++ b/www/asso_adhesion.xlsx
@@ -15,14 +15,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
   <si>
     <t>Id</t>
   </si>
   <si>
-    <t>Id_membre</t>
-  </si>
-  <si>
     <t>Prénom</t>
   </si>
   <si>
@@ -35,13 +32,28 @@
     <t>Date enregistrement</t>
   </si>
   <si>
-    <t>Veronique</t>
-  </si>
-  <si>
-    <t>Adragna</t>
-  </si>
-  <si>
-    <t>2019-04-16 12:39:10</t>
+    <t>Statut</t>
+  </si>
+  <si>
+    <t>Numéro de recu</t>
+  </si>
+  <si>
+    <t>celine</t>
+  </si>
+  <si>
+    <t>2019-06-21 12:30:53</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>R_2019_Adhesion_1004_celine_celine</t>
+  </si>
+  <si>
+    <t>2019-06-21 08:53:56</t>
+  </si>
+  <si>
+    <t>2019-06-20 14:58:16</t>
   </si>
 </sst>
 </file>
@@ -380,7 +392,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -388,7 +400,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -407,25 +419,71 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>300</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
         <v>9</v>
       </c>
-      <c r="B2">
-        <v>5984</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="E2">
-        <v>11111</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>987987</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>123</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mise en place page maintenance back , maj paiement validation temporaire, remerciement
</commit_message>
<xml_diff>
--- a/www/asso_adhesion.xlsx
+++ b/www/asso_adhesion.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="47">
   <si>
     <t>Id</t>
   </si>
@@ -38,22 +38,125 @@
     <t>Numéro de recu</t>
   </si>
   <si>
-    <t>celine</t>
+    <t>celine2</t>
+  </si>
+  <si>
+    <t>2019-06-27 15:01:33</t>
+  </si>
+  <si>
+    <t>WAIT</t>
+  </si>
+  <si>
+    <t>Aazzouz</t>
+  </si>
+  <si>
+    <t>Joelle</t>
+  </si>
+  <si>
+    <t>2019-06-23 14:02:44</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>2019-06-23 09:39:55</t>
+  </si>
+  <si>
+    <t>2019-06-23 09:39:22</t>
   </si>
   <si>
     <t>2019-06-21 12:30:53</t>
   </si>
   <si>
-    <t>OK</t>
-  </si>
-  <si>
-    <t>R_2019_Adhesion_1004_celine_celine</t>
+    <t>R_2019_Adhesion_1001_celine2_celine2</t>
   </si>
   <si>
     <t>2019-06-21 08:53:56</t>
   </si>
   <si>
-    <t>2019-06-20 14:58:16</t>
+    <t>2019-06-21 08:53:51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kern
+</t>
+  </si>
+  <si>
+    <t>Virginie</t>
+  </si>
+  <si>
+    <t>2019-06-18 13:29:13</t>
+  </si>
+  <si>
+    <t>2019-06-18 13:28:01</t>
+  </si>
+  <si>
+    <t>2019-06-05 09:20:36</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Linda</t>
+  </si>
+  <si>
+    <t>2019-04-16 12:49:15</t>
+  </si>
+  <si>
+    <t>2019-04-16 12:49:12</t>
+  </si>
+  <si>
+    <t>2019-04-16 12:49:09</t>
+  </si>
+  <si>
+    <t>2019-04-16 12:49:05</t>
+  </si>
+  <si>
+    <t>2019-04-16 12:49:03</t>
+  </si>
+  <si>
+    <t>2019-04-16 12:49:00</t>
+  </si>
+  <si>
+    <t>Adragna</t>
+  </si>
+  <si>
+    <t>Veronique</t>
+  </si>
+  <si>
+    <t>2019-04-16 12:39:10</t>
+  </si>
+  <si>
+    <t>Abramovici</t>
+  </si>
+  <si>
+    <t>Nello</t>
+  </si>
+  <si>
+    <t>2019-04-16 12:21:46</t>
+  </si>
+  <si>
+    <t>Achard</t>
+  </si>
+  <si>
+    <t>Guillaume</t>
+  </si>
+  <si>
+    <t>2019-04-16 12:03:14</t>
+  </si>
+  <si>
+    <t>Adamadorassy</t>
+  </si>
+  <si>
+    <t>Mickael</t>
+  </si>
+  <si>
+    <t>2019-04-16 11:46:32</t>
+  </si>
+  <si>
+    <t>2019-04-16 11:44:03</t>
+  </si>
+  <si>
+    <t>2019-04-16 11:43:44</t>
   </si>
 </sst>
 </file>
@@ -392,7 +495,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -425,7 +528,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -434,7 +537,7 @@
         <v>7</v>
       </c>
       <c r="D2">
-        <v>300</v>
+        <v>1000</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -442,47 +545,467 @@
       <c r="F2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D3">
-        <v>987987</v>
+        <v>1234</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4">
+        <v>37</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>654984</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>36</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5">
+        <v>32132</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>300</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <v>987987</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>54484</v>
+      </c>
+      <c r="E8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9">
+        <v>333</v>
+      </c>
+      <c r="E9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10">
+        <v>1321</v>
+      </c>
+      <c r="E10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11">
+        <v>30</v>
+      </c>
+      <c r="E11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>100</v>
+      </c>
+      <c r="E12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13">
+        <v>25</v>
+      </c>
+      <c r="E13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14">
+        <v>786782222</v>
+      </c>
+      <c r="E14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15">
+        <v>785786796</v>
+      </c>
+      <c r="E15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16">
+        <v>4153563</v>
+      </c>
+      <c r="E16" t="s">
         <v>29</v>
       </c>
-      <c r="B4" t="s">
+      <c r="F16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17">
+        <v>7878678</v>
+      </c>
+      <c r="E17" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18">
+        <v>7783893</v>
+      </c>
+      <c r="E18" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19">
+        <v>10</v>
+      </c>
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19">
+        <v>111111</v>
+      </c>
+      <c r="E19" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20">
+        <v>9</v>
+      </c>
+      <c r="B20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20">
+        <v>11111</v>
+      </c>
+      <c r="E20" t="s">
+        <v>35</v>
+      </c>
+      <c r="F20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21">
+        <v>8</v>
+      </c>
+      <c r="B21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21">
+        <v>456456</v>
+      </c>
+      <c r="E21" t="s">
+        <v>38</v>
+      </c>
+      <c r="F21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4">
-        <v>123</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="B22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22">
+        <v>33333</v>
+      </c>
+      <c r="E22" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23">
+        <v>6</v>
+      </c>
+      <c r="B23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23">
+        <v>12872</v>
+      </c>
+      <c r="E23" t="s">
+        <v>44</v>
+      </c>
+      <c r="F23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24">
+        <v>124</v>
+      </c>
+      <c r="E24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25">
+        <v>4</v>
+      </c>
+      <c r="B25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25">
+        <v>10000</v>
+      </c>
+      <c r="E25" t="s">
+        <v>46</v>
+      </c>
+      <c r="F25" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>